<commit_message>
ENHANCEMENT : enhance the logging and code quality on all scripts and correct the importations on template and correct the environement variables declaration.
</commit_message>
<xml_diff>
--- a/data/data-1.xlsx
+++ b/data/data-1.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\work\Code\Github\custom-pdf-generator\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E77208C-5AC9-4CE2-9203-62B2939EEE6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2385" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Column1</t>
   </si>
@@ -31,15 +25,21 @@
     <t>Column3</t>
   </si>
   <si>
+    <t>image</t>
+  </si>
+  <si>
     <t>Sample Text 1</t>
   </si>
   <si>
-    <t>Sample Text 2</t>
+    <t>Sample sadasdText 2</t>
   </si>
   <si>
     <t>Sample Text 3</t>
   </si>
   <si>
+    <t>assets/logo-1.png</t>
+  </si>
+  <si>
     <t>Sample Text 4</t>
   </si>
   <si>
@@ -49,12 +49,6 @@
     <t>Sample Text 6</t>
   </si>
   <si>
-    <t>path/to/image1.jpg</t>
-  </si>
-  <si>
-    <t>path/to/image2.jpg</t>
-  </si>
-  <si>
     <t>Sample Text 7</t>
   </si>
   <si>
@@ -62,19 +56,14 @@
   </si>
   <si>
     <t>Sample Text 9</t>
-  </si>
-  <si>
-    <t>path/to/image3.jpg</t>
-  </si>
-  <si>
-    <t>image</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,21 +73,15 @@
     </font>
     <font>
       <sz val="8"/>
-      <color rgb="FFF8FAFF"/>
+      <color rgb="FFf8faff"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FFF8FAFF"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -110,12 +93,33 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF292A2D"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FF292a2d"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFc6c6c6"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFc6c6c6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFc6c6c6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFc6c6c6"/>
+      </bottom>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -127,67 +131,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+  <cellXfs count="5">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FFF8FAFF"/>
-        <name val="Segoe UI"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF292A2D"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:D4" totalsRowShown="0">
-  <autoFilter ref="A1:D4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D4" displayName="Tableau1" name="Tableau1" id="1" totalsRowShown="0">
+  <autoFilter ref="A1:D4"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Column3"/>
-    <tableColumn id="4" xr3:uid="{CBF28273-B6A6-41D3-9180-12CB1A530FBE}" name="image" dataDxfId="0"/>
+    <tableColumn name="Column1" id="1"/>
+    <tableColumn name="Column2" id="2"/>
+    <tableColumn name="Column3" id="3"/>
+    <tableColumn name="image" id="4"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight1" showColumnStripes="0" showRowStripes="1" showLastColumn="0" showFirstColumn="0"/>
 </table>
 </file>
 
@@ -196,10 +177,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -237,71 +218,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -329,7 +310,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -352,11 +333,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -365,13 +346,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -381,7 +362,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -390,7 +371,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -399,7 +380,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -407,10 +388,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -475,65 +456,65 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33" customWidth="1"/>
+    <col min="1" max="1" style="4" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="33.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>15</v>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="23" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -544,11 +525,10 @@
         <v>13</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>